<commit_message>
Melhorias em metodos do UtilExcel
</commit_message>
<xml_diff>
--- a/orcamentoAlex Tavares.xlsx
+++ b/orcamentoAlex Tavares.xlsx
@@ -1088,7 +1088,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" ht="14.25" customHeight="true">
+    <row r="25">
       <c r="A25" s="18" t="s">
         <v>25</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="I25" s="26"/>
       <c r="J25" s="27"/>
     </row>
-    <row r="26" ht="14.25" customHeight="true">
+    <row r="26">
       <c r="A26" s="28" t="s">
         <v>25</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="I26" s="36"/>
       <c r="J26" s="37"/>
     </row>
-    <row r="27" ht="14.25" customHeight="true">
+    <row r="27">
       <c r="A27" s="38" t="s">
         <v>25</v>
       </c>
@@ -1130,7 +1130,7 @@
       <c r="I27" s="46"/>
       <c r="J27" s="47"/>
     </row>
-    <row r="28" ht="14.25" customHeight="true">
+    <row r="28">
       <c r="A28" s="48" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
       <c r="I28" s="56"/>
       <c r="J28" s="57"/>
     </row>
-    <row r="29" ht="14.25" customHeight="true">
+    <row r="29">
       <c r="A29" s="58" t="s">
         <v>25</v>
       </c>

</xml_diff>